<commit_message>
poprawki uczenie na 800 iter
</commit_message>
<xml_diff>
--- a/zad 2 - porownanie modeli oe.xlsx
+++ b/zad 2 - porownanie modeli oe.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam0\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia\SEM 7\SZAU\Projekt 2\matlab\SZAU---proj-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE071E1F-6542-44AF-ADAF-8B1215EA60F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183048C1-116D-4DB9-9C5C-C501CB3D2C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12720" xr2:uid="{9FCD2ACA-0029-43EF-B7A5-D4585549BE51}"/>
   </bookViews>
@@ -52,9 +52,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +77,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFDBDEE1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -93,13 +100,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -139,18 +146,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -465,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF8AC36-400C-42DA-BB59-982E0254AC9A}">
-  <dimension ref="B4:N15"/>
+  <dimension ref="B4:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,21 +498,21 @@
   <sheetData>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -548,41 +556,37 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>82.372107999999997</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>82.372122000000005</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>82.372127000000006</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>82.372118999999998</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>82.372118</v>
-      </c>
-      <c r="H6">
-        <f>SUM(C6:G6)/5</f>
-        <v>82.372118799999996</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>63.189793000000002</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>63.189793000000002</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>63.189793000000002</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <v>63.189793000000002</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>63.189793000000002</v>
       </c>
     </row>
@@ -590,210 +594,190 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="4">
-        <v>35.660567999999998</v>
-      </c>
-      <c r="D7" s="4">
-        <v>29.508326</v>
-      </c>
-      <c r="E7" s="6">
-        <v>25.456644000000001</v>
+      <c r="C7" s="3">
+        <v>80.851449000000002</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.127365</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.1701459999999999</v>
       </c>
       <c r="F7" s="4">
-        <v>59.188626999999997</v>
-      </c>
-      <c r="G7" s="4">
-        <v>29.697495</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H14" si="0">SUM(C7:G7)/5</f>
-        <v>35.902332000000001</v>
+        <v>1.1268050000000001</v>
+      </c>
+      <c r="G7" s="3">
+        <v>27.566713</v>
       </c>
       <c r="I7" s="1">
         <v>2</v>
       </c>
-      <c r="J7" s="4">
-        <v>24.932881999999999</v>
-      </c>
-      <c r="K7" s="4">
-        <v>17.66414</v>
-      </c>
-      <c r="L7" s="6">
-        <v>17.573160999999999</v>
+      <c r="J7" s="3">
+        <v>21.749949000000001</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1.0657000000000001</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1.06799</v>
       </c>
       <c r="M7" s="4">
-        <v>36.439006999999997</v>
-      </c>
-      <c r="N7" s="4">
-        <v>21.474395000000001</v>
+        <v>1.0734950000000001</v>
+      </c>
+      <c r="N7" s="3">
+        <v>17.466435000000001</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" s="6">
-        <v>3.2315719999999999</v>
-      </c>
-      <c r="D8" s="4">
-        <v>11.363443</v>
-      </c>
-      <c r="E8" s="4">
-        <v>7.053191</v>
-      </c>
-      <c r="F8" s="4">
-        <v>7.7437459999999998</v>
-      </c>
-      <c r="G8" s="4">
-        <v>14.077287</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>8.6938478000000003</v>
+      <c r="C8" s="4">
+        <v>0.63303900000000002</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.633266</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.63305</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.076611</v>
+      </c>
+      <c r="G8" s="3">
+        <v>96.595910000000003</v>
       </c>
       <c r="I8" s="1">
         <v>3</v>
       </c>
-      <c r="J8" s="6">
-        <v>2.408582</v>
-      </c>
-      <c r="K8" s="4">
-        <v>6.8100129999999996</v>
-      </c>
-      <c r="L8" s="4">
-        <v>4.3265859999999998</v>
-      </c>
-      <c r="M8" s="4">
-        <v>4.2191400000000003</v>
-      </c>
-      <c r="N8" s="4">
-        <v>9.7125620000000001</v>
+      <c r="J8" s="4">
+        <v>0.37962299999999999</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.37962299999999999</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.37962299999999999</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.91695499999999996</v>
+      </c>
+      <c r="N8" s="3">
+        <v>10.097567</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="6">
-        <v>1.8299799999999999</v>
+      <c r="C9" s="3">
+        <v>0.34953800000000002</v>
       </c>
       <c r="D9" s="4">
-        <v>3.2989519999999999</v>
-      </c>
-      <c r="E9" s="4">
-        <v>5.2266830000000004</v>
-      </c>
-      <c r="F9" s="4">
-        <v>11.423788999999999</v>
-      </c>
-      <c r="G9" s="4">
-        <v>2.2301989999999998</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>4.8019205999999999</v>
+        <v>0.33283099999999999</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.44321500000000003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.66923900000000003</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.35732000000000003</v>
       </c>
       <c r="I9" s="1">
         <v>4</v>
       </c>
-      <c r="J9" s="6">
-        <v>0.65842500000000004</v>
+      <c r="J9" s="3">
+        <v>0.18673600000000001</v>
       </c>
       <c r="K9" s="4">
-        <v>1.642144</v>
-      </c>
-      <c r="L9" s="4">
-        <v>3.0398839999999998</v>
-      </c>
-      <c r="M9" s="4">
-        <v>7.7819789999999998</v>
-      </c>
-      <c r="N9" s="4">
-        <v>1.9875290000000001</v>
+        <v>0.22708400000000001</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.27618199999999998</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.19916500000000001</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.230041</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
-      <c r="C10" s="4">
-        <v>5.9547020000000002</v>
-      </c>
-      <c r="D10" s="4">
-        <v>2.8015089999999998</v>
-      </c>
-      <c r="E10" s="4">
-        <v>3.2763520000000002</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1.2410509999999999</v>
-      </c>
-      <c r="G10" s="4">
-        <v>3.2763520000000002</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
-        <v>3.3099932000000001</v>
+      <c r="C10" s="3">
+        <v>0.78175700000000004</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.190194</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2.2605059999999999</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.16290099999999999</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.58446799999999999</v>
       </c>
       <c r="I10" s="1">
         <v>5</v>
       </c>
-      <c r="J10" s="4">
-        <v>3.30985</v>
-      </c>
-      <c r="K10" s="4">
-        <v>1.5415140000000001</v>
-      </c>
-      <c r="L10" s="4">
-        <v>2.0982229999999999</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0.72550199999999998</v>
-      </c>
-      <c r="N10" s="4">
-        <v>2.0982229999999999</v>
+      <c r="J10" s="3">
+        <v>0.15798000000000001</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.126416</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.13195899999999999</v>
+      </c>
+      <c r="M10" s="4">
+        <v>7.1964E-2</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.18523400000000001</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6</v>
       </c>
-      <c r="C11" s="4">
-        <v>3.6300063147641399</v>
-      </c>
-      <c r="D11" s="4">
-        <v>6.3851871365130002</v>
-      </c>
-      <c r="E11" s="4">
-        <v>2.8999539462825501</v>
+      <c r="C11" s="3">
+        <v>0.41968451840131199</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.36139470764445097</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.21252828056853201</v>
       </c>
       <c r="F11" s="4">
-        <v>2.99604541383985</v>
-      </c>
-      <c r="G11" s="6">
-        <v>1.8108934005576101</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
-        <v>3.5444172423914297</v>
+        <v>0.110701401592221</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.34031942237159402</v>
       </c>
       <c r="I11" s="1">
         <v>6</v>
       </c>
-      <c r="J11" s="4">
-        <v>2.7889153322758098</v>
-      </c>
-      <c r="K11" s="4">
-        <v>3.9186245459269902</v>
-      </c>
-      <c r="L11" s="4">
-        <v>1.89184824627464</v>
+      <c r="J11" s="3">
+        <v>6.6573210173162006E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.15522056051095001</v>
+      </c>
+      <c r="L11" s="3">
+        <v>5.8535631897189001E-2</v>
       </c>
       <c r="M11" s="4">
-        <v>2.4421372254782301</v>
-      </c>
-      <c r="N11" s="6">
-        <v>1.10737831775475</v>
+        <v>4.9996985256814001E-2</v>
+      </c>
+      <c r="N11" s="3">
+        <v>5.2145237647545001E-2</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -801,168 +785,155 @@
         <v>7</v>
       </c>
       <c r="C12" s="4">
-        <v>1.3380471547230499</v>
-      </c>
-      <c r="D12" s="4">
-        <v>2.6627818084619599</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1.17342593751257</v>
-      </c>
-      <c r="F12" s="4">
-        <v>3.8190543109872701</v>
-      </c>
-      <c r="G12" s="4">
-        <v>4.4298027555236503</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>2.6846223934416997</v>
+        <v>9.7816970438338993E-2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.20417089397919999</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.15854527693084899</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.28439349493231197</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.33256892298433799</v>
       </c>
       <c r="I12" s="1">
         <v>7</v>
       </c>
       <c r="J12" s="4">
-        <v>0.96715924842540202</v>
-      </c>
-      <c r="K12" s="4">
-        <v>1.5399587380928199</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0.81294305477231499</v>
-      </c>
-      <c r="M12" s="4">
-        <v>2.38757602119124</v>
-      </c>
-      <c r="N12" s="4">
-        <v>2.81616463486451</v>
+        <v>5.2563623051589001E-2</v>
+      </c>
+      <c r="K12" s="3">
+        <v>8.7377785673321995E-2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>8.9760386912362003E-2</v>
+      </c>
+      <c r="M12" s="3">
+        <v>5.7919019261172003E-2</v>
+      </c>
+      <c r="N12" s="3">
+        <v>2.4160005267326E-2</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>8</v>
       </c>
-      <c r="C13" s="4">
-        <v>1.52006814083287</v>
-      </c>
-      <c r="D13" s="6">
-        <v>1.2619282185448999</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2.67525010681979</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1.13717148858825</v>
-      </c>
-      <c r="G13" s="4">
-        <v>4.3262623897264296</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="0"/>
-        <v>2.1841360689024478</v>
+      <c r="C13" s="3">
+        <v>0.28873925056157401</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.33035339746040898</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1.6451E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3.8631022400280997E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.125576092985695</v>
       </c>
       <c r="I13" s="1">
         <v>8</v>
       </c>
-      <c r="J13" s="4">
-        <v>0.99027501292761799</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0.91545508381298502</v>
-      </c>
-      <c r="L13" s="4">
-        <v>1.0092570289737699</v>
-      </c>
-      <c r="M13" s="6">
-        <v>0.74557510073932398</v>
-      </c>
-      <c r="N13" s="4">
-        <v>2.96437156784003</v>
+      <c r="J13" s="3">
+        <v>6.8321769916374994E-2</v>
+      </c>
+      <c r="K13" s="3">
+        <v>5.57506345137E-2</v>
+      </c>
+      <c r="L13" s="5">
+        <v>9.469E-3</v>
+      </c>
+      <c r="M13" s="3">
+        <v>2.0762357195544E-2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>4.3296088494143001E-2</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>9</v>
       </c>
-      <c r="C14" s="4">
-        <v>2.3122377173884301</v>
-      </c>
-      <c r="D14" s="6">
-        <v>1.31785265201144</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1.7050396256864899</v>
+      <c r="C14" s="3">
+        <v>0.13824620400321599</v>
+      </c>
+      <c r="D14" s="3">
+        <v>7.7772859023525001E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7.4736952051976002E-2</v>
       </c>
       <c r="F14" s="4">
-        <v>1.37847506170175</v>
-      </c>
-      <c r="G14" s="4">
-        <v>2.4060036808790501</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="0"/>
-        <v>1.8239217475334322</v>
+        <v>4.5920369455891001E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>6.4323567056665004E-2</v>
       </c>
       <c r="I14" s="1">
         <v>9</v>
       </c>
-      <c r="J14" s="4">
-        <v>1.6517629509071501</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0.94666229656392398</v>
-      </c>
-      <c r="L14" s="4">
-        <v>1.3361471805012799</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0.82619050209724498</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1.3512202042179999</v>
+      <c r="J14" s="3">
+        <v>2.2474258815817001E-2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2.4267746862770001E-2</v>
+      </c>
+      <c r="L14" s="3">
+        <v>4.1171222647002001E-2</v>
+      </c>
+      <c r="M14" s="4">
+        <v>2.3096358641756999E-2</v>
+      </c>
+      <c r="N14" s="3">
+        <v>2.4112426810951999E-2</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>10</v>
       </c>
-      <c r="C15" s="4">
-        <v>1.62896852565523</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1.2503642497459799</v>
+      <c r="C15" s="3">
+        <v>0.23712800000000001</v>
+      </c>
+      <c r="D15" s="3">
+        <v>4.6486E-2</v>
       </c>
       <c r="E15" s="4">
-        <v>2.4756498408256098</v>
-      </c>
-      <c r="F15" s="4">
-        <v>1.7670570443909599</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1.1359750713203001</v>
-      </c>
-      <c r="H15">
-        <f>SUM(C15:G15)/5</f>
-        <v>1.6516029463876158</v>
+        <v>4.2084999999999997E-2</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.10992399999999999</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.68898417439488902</v>
       </c>
       <c r="I15" s="2">
         <v>10</v>
       </c>
-      <c r="J15" s="4">
-        <v>0.88656661617953803</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0.97435605025707195</v>
+      <c r="J15" s="3">
+        <v>2.7165000000000002E-2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3.3188000000000002E-2</v>
       </c>
       <c r="L15" s="4">
-        <v>1.3796222889087599</v>
-      </c>
-      <c r="M15" s="4">
-        <v>0.90716391835992105</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0.56691398772384405</v>
-      </c>
+        <v>1.7305999999999998E-2</v>
+      </c>
+      <c r="M15" s="3">
+        <v>6.7039999999999999E-3</v>
+      </c>
+      <c r="N15" s="3">
+        <v>1.8795257371510998E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -971,5 +942,6 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>